<commit_message>
WIP Targeted Data Strategy examples
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data-management/artifact/data/PlanControl1.data.xlsx
+++ b/examples/data-management/artifact/data/PlanControl1.data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ml093043/projects/nexial/nexial-core/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lium183/projects/nexial/tutorials/examples/data-management/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4D5852-A8B1-6542-8E07-69F7FEC0612B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7897CDD0-E2A9-C24F-B2FF-E509F7B65089}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="25140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="9340" windowWidth="25600" windowHeight="15760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="#default" sheetId="2" r:id="rId1"/>
@@ -49,21 +49,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>true</t>
   </si>
   <si>
-    <t>800</t>
-  </si>
-  <si>
-    <t>,</t>
-  </si>
-  <si>
     <t>1</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
   <si>
     <t>nexial.scope.fallbackToPrevious</t>
@@ -72,19 +63,16 @@
     <t>nexial.scope.iteration</t>
   </si>
   <si>
-    <t>nexial.pollWaitMs</t>
+    <t>MyTest.BusinessName</t>
   </si>
   <si>
-    <t>nexial.failFast</t>
+    <t>Acme Hardware</t>
   </si>
   <si>
-    <t>nexial.textDelim</t>
+    <t>MyTest.BusinessOpensOn</t>
   </si>
   <si>
-    <t>nexial.verbose</t>
-  </si>
-  <si>
-    <t>nexial.openResult</t>
+    <t>Monday through Saturday</t>
   </si>
 </sst>
 </file>
@@ -600,11 +588,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AAA200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="23.7109375" style="5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="21.28515625" style="4" customWidth="1" collapsed="1"/>
     <col min="3" max="52" width="21.28515625" style="2" customWidth="1" collapsed="1"/>
     <col min="53" max="16384" width="10.7109375" style="2" collapsed="1"/>
@@ -612,7 +602,7 @@
   <sheetData>
     <row r="1" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -622,61 +612,46 @@
     </row>
     <row r="2" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="HA2" s="3"/>
       <c r="AAA2" s="3"/>
     </row>
     <row r="3" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="HA3" s="3"/>
       <c r="AAA3" s="3"/>
     </row>
     <row r="4" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="HA4" s="6"/>
       <c r="AAA4" s="7"/>
     </row>
     <row r="5" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>2</v>
-      </c>
+      <c r="A5" s="1"/>
       <c r="HA5" s="6"/>
       <c r="AAA5" s="7"/>
     </row>
     <row r="6" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="HA6" s="6"/>
       <c r="AAA6" s="7"/>
     </row>
     <row r="7" spans="1:703" ht="23" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>0</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="HA7" s="6"/>
       <c r="AAA7" s="7"/>
     </row>

</xml_diff>

<commit_message>
WIP - Targeted Data Management
Signed-off-by: automike <mikeliucc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data-management/artifact/data/PlanControl1.data.xlsx
+++ b/examples/data-management/artifact/data/PlanControl1.data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lium183/projects/nexial/tutorials/examples/data-management/artifact/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7897CDD0-E2A9-C24F-B2FF-E509F7B65089}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9190AF-48D7-4445-80AF-D74FF6D4FF2D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="9340" windowWidth="25600" windowHeight="15760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,16 +63,16 @@
     <t>nexial.scope.iteration</t>
   </si>
   <si>
-    <t>MyTest.BusinessName</t>
+    <t>MyTest.BusinessStarts</t>
   </si>
   <si>
-    <t>Acme Hardware</t>
+    <t>08:00</t>
   </si>
   <si>
-    <t>MyTest.BusinessOpensOn</t>
+    <t>MyTest.BusinessCloses</t>
   </si>
   <si>
-    <t>Monday through Saturday</t>
+    <t>21:00</t>
   </si>
 </sst>
 </file>
@@ -589,7 +589,7 @@
   <dimension ref="A1:AAA200"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A3" sqref="A3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0.25"/>

</xml_diff>